<commit_message>
+updated: list of known diagnosed cases --> This is based on feedback and advice from the ORTHO & PT unit member. --> work-in-progress
</commit_message>
<xml_diff>
--- a/generateMonthlySummaryReport/add-on software/assets/diagnosedCasesList.xlsx
+++ b/generateMonthlySummaryReport/add-on software/assets/diagnosedCasesList.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="diagnosedCasesList" localSheetId="0">Sheet1!$A$1:$B$88</definedName>
+    <definedName name="diagnosedCasesList" localSheetId="0">Sheet1!$A$1:$B$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
   <si>
     <t>Classification</t>
   </si>
@@ -326,13 +326,16 @@
     <t>Calcific Tendinitis</t>
   </si>
   <si>
-    <t>HNP</t>
-  </si>
-  <si>
     <t>Iliotibial Band Syndrome</t>
   </si>
   <si>
     <t>Patello Femoral Pain Syndrome</t>
+  </si>
+  <si>
+    <t>Tendinitis</t>
+  </si>
+  <si>
+    <t>impingement</t>
   </si>
 </sst>
 </file>
@@ -654,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +842,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,7 +850,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,10 +1143,10 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1154,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1162,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,7 +1170,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1178,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,15 +1186,15 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1202,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1210,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1218,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1223,7 +1226,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1234,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,47 +1242,47 @@
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1287,15 +1290,15 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1303,7 +1306,7 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1311,7 +1314,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1319,7 +1322,7 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,7 +1330,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1335,7 +1338,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,30 +1346,46 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>90</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+updated: instructions to process the list of known diagnosed cases from the top row to the bottom row --> At present, the add-on computer software stops processing the list as soon as it identifies a classification for the input diagnosis. --> Therefore, a unit member must write cases in the list in order of priority with the top given the highest priority. --> work-in-progress
</commit_message>
<xml_diff>
--- a/generateMonthlySummaryReport/add-on software/assets/diagnosedCasesList.xlsx
+++ b/generateMonthlySummaryReport/add-on software/assets/diagnosedCasesList.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="diagnosedCasesList" localSheetId="0">Sheet1!$A$1:$B$90</definedName>
+    <definedName name="diagnosedCasesList" localSheetId="0">Sheet1!$A$1:$B$91</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="100">
   <si>
     <t>Classification</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>impingement</t>
+  </si>
+  <si>
+    <t>FX Lumbar</t>
   </si>
 </sst>
 </file>
@@ -657,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,10 +1146,10 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1154,7 +1157,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1165,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1173,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1178,7 +1181,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,15 +1189,15 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1205,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1213,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1221,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1226,7 +1229,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,7 +1237,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,47 +1245,47 @@
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1290,15 +1293,15 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1306,7 +1309,7 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,7 +1317,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1322,7 +1325,7 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1330,7 +1333,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1338,7 +1341,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1349,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1357,7 @@
         <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,23 +1365,23 @@
         <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,6 +1389,14 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>